<commit_message>
Add further unit tests and fix issues found when reviewing code
</commit_message>
<xml_diff>
--- a/tests/fixtures/matrix_sample.xlsx
+++ b/tests/fixtures/matrix_sample.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="278">
   <si>
     <t xml:space="preserve">Contexte</t>
   </si>
@@ -1195,6 +1195,9 @@
     <t xml:space="preserve">ruminants, chien, chat  </t>
   </si>
   <si>
+    <t xml:space="preserve">CoPrev.1.1bis.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Réaliser un examen comportemental sur un groupe d’animaux </t>
   </si>
   <si>
@@ -1222,7 +1225,7 @@
     <t xml:space="preserve">Juger de l’état d’entretien d’un animal ou d’un groupe d’animaux</t>
   </si>
   <si>
-    <t xml:space="preserve">CoPrev 1.4.</t>
+    <t xml:space="preserve">CoPrev.1.4.</t>
   </si>
   <si>
     <t xml:space="preserve">Réaliser une diagnose de catégorie et une évaluation comportementale dans le cadre de la réglementation liée aux chiens susceptibles d'être dangereux  </t>
@@ -1276,7 +1279,7 @@
     <t xml:space="preserve">chien, chat, cheval, ruminants</t>
   </si>
   <si>
-    <t xml:space="preserve">CoPrev 2.5.</t>
+    <t xml:space="preserve">CoPrev.2.5.</t>
   </si>
   <si>
     <t xml:space="preserve">Conseiller un utilisateur d’animal de sport ou d’utilité sur les éléments de prévention spécifiques  </t>
@@ -1336,7 +1339,7 @@
     <t xml:space="preserve">Appliquer les principes et les méthodes pour éliminer les cadavres, les sous-produits animaux, et les déchets d'activité de soins dans le respect de la réglementation et des règles de biosécurité</t>
   </si>
   <si>
-    <t xml:space="preserve">Coprev 3.4.</t>
+    <t xml:space="preserve">Coprev.3.4.</t>
   </si>
   <si>
     <t xml:space="preserve">Justifier, appliquer et faire appliquer les mesures de biosécurité face à un incident de nature à mettre en jeu la sécurité sanitaire des personnes ou des animaux  </t>
@@ -1462,55 +1465,55 @@
     <t xml:space="preserve">Effectuer un prélèvement biologique </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.01.</t>
+    <t xml:space="preserve">D.3.2bis.01.</t>
   </si>
   <si>
     <t xml:space="preserve">Prélèvement sanguin</t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.02.</t>
+    <t xml:space="preserve">D.3.2bis.02.</t>
   </si>
   <si>
     <t xml:space="preserve">Prélèvement de lait</t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.03.</t>
+    <t xml:space="preserve">D.3.2bis.03.</t>
   </si>
   <si>
     <t xml:space="preserve">Prélèvement de semence</t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.04.</t>
+    <t xml:space="preserve">D.3.2bis.04.</t>
   </si>
   <si>
     <t xml:space="preserve">Prélèvements de matières fécales </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.05.</t>
+    <t xml:space="preserve">D.3.2bis.05.</t>
   </si>
   <si>
     <t xml:space="preserve">Prélèvement d’urine </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.06.</t>
+    <t xml:space="preserve">D.3.2bis.06.</t>
   </si>
   <si>
     <t xml:space="preserve">Écouvillonnages </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.07.</t>
+    <t xml:space="preserve">D.3.2bis.07.</t>
   </si>
   <si>
     <t xml:space="preserve">Raclage cutané </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.08.</t>
+    <t xml:space="preserve">D.3.2bis.08.</t>
   </si>
   <si>
     <t xml:space="preserve">Aspiration transtrachéale et lavage broncho alvéolaire </t>
   </si>
   <si>
-    <t xml:space="preserve"> D.3.2bis.09.</t>
+    <t xml:space="preserve">D.3.2bis.09.</t>
   </si>
   <si>
     <t xml:space="preserve">Cytoponctions superficielles et ponctions de liquides biologiques (articulaire, épanchement abdominal et thoracique) </t>
@@ -1573,7 +1576,10 @@
     <t xml:space="preserve">espèces majeures</t>
   </si>
   <si>
-    <t xml:space="preserve">bis Choisir la technique d'imagerie la plus adaptée au contexte clinique (hypothèses diagnostiques, contexte socio-économique, principe de justification, limites, contre-indications) (radio-écho-scanner-IRM-scintigraphie)  </t>
+    <t xml:space="preserve">D.4.1bis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choisir la technique d'imagerie la plus adaptée au contexte clinique (hypothèses diagnostiques, contexte socio-économique, principe de justification, limites, contre-indications) (radio-écho-scanner-IRM-scintigraphie)  </t>
   </si>
   <si>
     <t xml:space="preserve">D.4.2.</t>
@@ -1585,10 +1591,16 @@
     <t xml:space="preserve">chien, chat / autres espèces</t>
   </si>
   <si>
-    <t xml:space="preserve">bis Réaliser un cliché radiographique :  examen radiographique avec produit de contraste</t>
+    <t xml:space="preserve">D.4.2bis.</t>
   </si>
   <si>
-    <t xml:space="preserve">ter Réaliser un cliché radiographique :  principales incidences radiographiques </t>
+    <t xml:space="preserve">Réaliser un cliché radiographique :  examen radiographique avec produit de contraste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.4.2ter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réaliser un cliché radiographique :  principales incidences radiographiques </t>
   </si>
   <si>
     <t xml:space="preserve">D.4.3.</t>
@@ -1600,13 +1612,19 @@
     <t xml:space="preserve">chien, chat cheval</t>
   </si>
   <si>
-    <t xml:space="preserve">bis Réaliser un examen échographique :  échographie de l’appareil génital de la vache </t>
+    <t xml:space="preserve">D.4.3bis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réaliser un examen échographique :  échographie de l’appareil génital de la vache </t>
   </si>
   <si>
     <t xml:space="preserve">bovin</t>
   </si>
   <si>
-    <t xml:space="preserve">ter Réaliser un examen échographique :  échographie abdominale durant un examen de coliques, échographie de l’appareil génital chez la jument </t>
+    <t xml:space="preserve">D.4.3ter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réaliser un examen échographique :  échographie abdominale durant un examen de coliques, échographie de l’appareil génital chez la jument </t>
   </si>
   <si>
     <t xml:space="preserve">D.4.4.</t>
@@ -1662,7 +1680,7 @@
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1927,13 +1945,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -2124,7 +2135,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2473,14 +2484,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17487,9 +17490,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1498680</xdr:colOff>
+      <xdr:colOff>1496160</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17504,7 +17507,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1498680" cy="4608000"/>
+          <a:ext cx="1496160" cy="4605480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17525,9 +17528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>7113240</xdr:colOff>
+      <xdr:colOff>7110720</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -17541,7 +17544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13436280" y="704880"/>
-          <a:ext cx="7062480" cy="9568080"/>
+          <a:ext cx="7059960" cy="9565560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -17563,7 +17566,7 @@
   </sheetPr>
   <dimension ref="B1:E79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -17877,7 +17880,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -18073,7 +18076,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -18269,8 +18272,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20629,22 +20632,22 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C7" s="66" t="n">
         <f aca="false">IF(OR(H7&lt;=1,I7&lt;=1)=1,0,IF(OR(H7&lt;2,I7&lt;2)=1,1,2))</f>
         <v>1</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G7" s="67" t="n">
         <f aca="false">COUNTIF(N7:HA7,1)+COUNTIF(N7:HA7,2)*0.5</f>
@@ -21203,20 +21206,20 @@
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C8" s="66" t="n">
         <f aca="false">IF(OR(H8&lt;=1,I8&lt;=1)=1,0,IF(OR(H8&lt;2,I8&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G8" s="67" t="n">
         <f aca="false">COUNTIF(N8:HA8,1)+COUNTIF(N8:HA8,2)*0.5</f>
@@ -21775,20 +21778,20 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C9" s="66" t="n">
         <f aca="false">IF(OR(H9&lt;=1,I9&lt;=1)=1,0,IF(OR(H9&lt;2,I9&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D9" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G9" s="67" t="n">
         <f aca="false">COUNTIF(N9:HA9,1)+COUNTIF(N9:HA9,2)*0.5</f>
@@ -22345,22 +22348,22 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C10" s="66" t="n">
         <f aca="false">IF(OR(H10&lt;=1,I10&lt;=1)=1,0,IF(OR(H10&lt;2,I10&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G10" s="67" t="n">
         <f aca="false">COUNTIF(N10:HA10,1)+COUNTIF(N10:HA10,2)*0.5</f>
@@ -22919,10 +22922,10 @@
     </row>
     <row r="11" s="71" customFormat="true" ht="72.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="60" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" s="66"/>
       <c r="D11" s="69"/>
@@ -23470,17 +23473,17 @@
     </row>
     <row r="12" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C12" s="66" t="n">
         <f aca="false">IF(OR(H12&lt;=1,I12&lt;=1)=1,0,IF(OR(H12&lt;2,I12&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F12" s="48"/>
       <c r="G12" s="67" t="n">
@@ -24040,20 +24043,20 @@
     </row>
     <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C13" s="66" t="n">
         <f aca="false">IF(OR(H13&lt;=1,I13&lt;=1)=1,0,IF(OR(H13&lt;2,I13&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G13" s="67" t="n">
         <f aca="false">COUNTIF(N13:HA13,1)+COUNTIF(N13:HA13,2)*0.5</f>
@@ -24612,20 +24615,20 @@
     </row>
     <row r="14" customFormat="false" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C14" s="66" t="n">
         <f aca="false">IF(OR(H14&lt;=1,I14&lt;=1)=1,0,IF(OR(H14&lt;2,I14&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G14" s="67" t="n">
         <f aca="false">COUNTIF(N14:HA14,1)+COUNTIF(N14:HA14,2)*0.5</f>
@@ -25184,20 +25187,20 @@
     </row>
     <row r="15" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C15" s="66" t="n">
         <f aca="false">IF(OR(H15&lt;=1,I15&lt;=1)=1,0,IF(OR(H15&lt;2,I15&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F15" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G15" s="67" t="n">
         <f aca="false">COUNTIF(N15:HA15,1)+COUNTIF(N15:HA15,2)*0.5</f>
@@ -25756,20 +25759,20 @@
     </row>
     <row r="16" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C16" s="66" t="n">
         <f aca="false">IF(OR(H16&lt;=1,I16&lt;=1)=1,0,IF(OR(H16&lt;2,I16&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G16" s="67" t="n">
         <f aca="false">COUNTIF(N16:HA16,1)+COUNTIF(N16:HA16,2)*0.5</f>
@@ -26326,22 +26329,22 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C17" s="66" t="n">
         <f aca="false">IF(OR(H17&lt;=1,I17&lt;=1)=1,0,IF(OR(H17&lt;2,I17&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G17" s="67" t="n">
         <f aca="false">COUNTIF(N17:HA17,1)+COUNTIF(N17:HA17,2)*0.5</f>
@@ -26900,20 +26903,20 @@
     </row>
     <row r="18" customFormat="false" ht="54.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C18" s="66" t="n">
         <f aca="false">IF(OR(H18&lt;=1,I18&lt;=1)=1,0,IF(OR(H18&lt;2,I18&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F18" s="48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G18" s="67" t="n">
         <f aca="false">COUNTIF(N18:HA18,1)+COUNTIF(N18:HA18,2)*0.5</f>
@@ -27472,10 +27475,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C19" s="66" t="n">
         <f aca="false">IF(OR(H19&lt;=1,I19&lt;=1)=1,0,IF(OR(H19&lt;2,I19&lt;2)=1,1,2))</f>
@@ -27485,7 +27488,7 @@
         <v>118</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G19" s="67" t="n">
         <f aca="false">COUNTIF(N19:HA19,1)+COUNTIF(N19:HA19,2)*0.5</f>
@@ -28044,20 +28047,20 @@
     </row>
     <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C20" s="66" t="n">
         <f aca="false">IF(OR(H20&lt;=1,I20&lt;=1)=1,0,IF(OR(H20&lt;2,I20&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D20" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G20" s="67" t="n">
         <f aca="false">COUNTIF(N20:HA20,1)+COUNTIF(N20:HA20,2)*0.5</f>
@@ -28616,20 +28619,20 @@
     </row>
     <row r="21" customFormat="false" ht="54.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C21" s="66" t="n">
         <f aca="false">IF(OR(H21&lt;=1,I21&lt;=1)=1,0,IF(OR(H21&lt;2,I21&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F21" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G21" s="67" t="n">
         <f aca="false">COUNTIF(N21:HA21,1)+COUNTIF(N21:HA21,2)*0.5</f>
@@ -29188,10 +29191,10 @@
     </row>
     <row r="22" s="71" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="60" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C22" s="66"/>
       <c r="D22" s="72"/>
@@ -29739,10 +29742,10 @@
     </row>
     <row r="23" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C23" s="66" t="n">
         <f aca="false">IF(OR(H23&lt;=1,I23&lt;=1)=1,0,IF(OR(H23&lt;2,I23&lt;2)=1,1,2))</f>
@@ -29752,7 +29755,7 @@
         <v>118</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G23" s="67" t="n">
         <f aca="false">COUNTIF(N23:HA23,1)+COUNTIF(N23:HA23,2)*0.5</f>
@@ -30311,20 +30314,20 @@
     </row>
     <row r="24" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C24" s="66" t="n">
         <f aca="false">IF(OR(H24&lt;=1,I24&lt;=1)=1,0,IF(OR(H24&lt;2,I24&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G24" s="67" t="n">
         <f aca="false">COUNTIF(N24:HA24,1)+COUNTIF(N24:HA24,2)*0.5</f>
@@ -30883,10 +30886,10 @@
     </row>
     <row r="25" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C25" s="66" t="n">
         <f aca="false">IF(OR(H25&lt;=1,I25&lt;=1)=1,0,IF(OR(H25&lt;2,I25&lt;2)=1,1,2))</f>
@@ -30896,7 +30899,7 @@
         <v>118</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G25" s="67" t="n">
         <f aca="false">COUNTIF(N25:HA25,1)+COUNTIF(N25:HA25,2)*0.5</f>
@@ -31453,22 +31456,22 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C26" s="66" t="n">
         <f aca="false">IF(OR(H26&lt;=1,I26&lt;=1)=1,0,IF(OR(H26&lt;2,I26&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F26" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G26" s="67" t="n">
         <f aca="false">COUNTIF(N26:HA26,1)+COUNTIF(N26:HA26,2)*0.5</f>
@@ -32027,10 +32030,10 @@
     </row>
     <row r="27" customFormat="false" ht="42.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="73" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C27" s="74"/>
       <c r="D27" s="75"/>
@@ -32247,10 +32250,10 @@
     </row>
     <row r="28" s="71" customFormat="true" ht="44.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="60" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C28" s="79"/>
       <c r="D28" s="69"/>
@@ -32638,10 +32641,10 @@
     </row>
     <row r="29" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C29" s="79" t="n">
         <f aca="false">IF(OR(H29&lt;=1,I29&lt;=1)=1,0,IF(OR(H29&lt;2,I29&lt;2)=1,1,2))</f>
@@ -32651,7 +32654,7 @@
         <v>118</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G29" s="67" t="n">
         <f aca="false">COUNTIF(N29:HA29,1)+COUNTIF(N29:HA29,2)*0.5</f>
@@ -33218,20 +33221,20 @@
     </row>
     <row r="30" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C30" s="79" t="n">
         <f aca="false">IF(OR(H30&lt;=1,I30&lt;=1)=1,0,IF(OR(H30&lt;2,I30&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G30" s="67" t="n">
         <f aca="false">COUNTIF(N30:HA30,1)+COUNTIF(N30:HA30,2)*0.5</f>
@@ -33798,20 +33801,20 @@
     </row>
     <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C31" s="79" t="n">
         <f aca="false">IF(OR(H31&lt;=1,I31&lt;=1)=1,0,IF(OR(H31&lt;2,I31&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F31" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G31" s="67" t="n">
         <f aca="false">COUNTIF(N31:HA31,1)+COUNTIF(N31:HA31,2)*0.5</f>
@@ -34378,20 +34381,20 @@
     </row>
     <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C32" s="79" t="n">
         <f aca="false">IF(OR(H32&lt;=1,I32&lt;=1)=1,0,IF(OR(H32&lt;2,I32&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F32" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G32" s="67" t="n">
         <f aca="false">COUNTIF(N32:HA32,1)+COUNTIF(N32:HA32,2)*0.5</f>
@@ -34958,10 +34961,10 @@
     </row>
     <row r="33" s="71" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="60" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B33" s="61" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C33" s="79"/>
       <c r="D33" s="69"/>
@@ -35517,20 +35520,20 @@
     </row>
     <row r="34" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C34" s="79" t="n">
         <f aca="false">IF(OR(H34&lt;=1,I34&lt;=1)=1,0,IF(OR(H34&lt;2,I34&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F34" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G34" s="67" t="n">
         <f aca="false">COUNTIF(N34:HA34,1)+COUNTIF(N34:HA34,2)*0.5</f>
@@ -36097,10 +36100,10 @@
     </row>
     <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C35" s="79" t="n">
         <f aca="false">IF(OR(H35&lt;=1,I35&lt;=1)=1,0,IF(OR(H35&lt;2,I35&lt;2)=1,1,2))</f>
@@ -36110,7 +36113,7 @@
         <v>118</v>
       </c>
       <c r="F35" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G35" s="67" t="n">
         <f aca="false">COUNTIF(N35:HA35,1)+COUNTIF(N35:HA35,2)*0.5</f>
@@ -36677,20 +36680,20 @@
     </row>
     <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C36" s="79" t="n">
         <f aca="false">IF(OR(H36&lt;=1,I36&lt;=1)=1,0,IF(OR(H36&lt;2,I36&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F36" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G36" s="67" t="n">
         <f aca="false">COUNTIF(N36:HA36,1)+COUNTIF(N36:HA36,2)*0.5</f>
@@ -37257,20 +37260,20 @@
     </row>
     <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C37" s="79" t="n">
         <f aca="false">IF(OR(H37&lt;=1,I37&lt;=1)=1,0,IF(OR(H37&lt;2,I37&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F37" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G37" s="67" t="n">
         <f aca="false">COUNTIF(N37:HA37,1)+COUNTIF(N37:HA37,2)*0.5</f>
@@ -37837,20 +37840,20 @@
     </row>
     <row r="38" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C38" s="79" t="n">
         <f aca="false">IF(OR(H38&lt;=1,I38&lt;=1)=1,0,IF(OR(H38&lt;2,I38&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G38" s="67" t="n">
         <f aca="false">COUNTIF(N38:HA38,1)+COUNTIF(N38:HA38,2)*0.5</f>
@@ -38417,20 +38420,20 @@
     </row>
     <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C39" s="79" t="n">
         <f aca="false">IF(OR(H39&lt;=1,I39&lt;=1)=1,0,IF(OR(H39&lt;2,I39&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F39" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G39" s="67" t="n">
         <f aca="false">COUNTIF(N39:HA39,1)+COUNTIF(N39:HA39,2)*0.5</f>
@@ -38997,10 +39000,10 @@
     </row>
     <row r="40" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C40" s="79" t="n">
         <f aca="false">IF(OR(H40&lt;=1,I40&lt;=1)=1,0,IF(OR(H40&lt;2,I40&lt;2)=1,1,2))</f>
@@ -39010,7 +39013,7 @@
         <v>118</v>
       </c>
       <c r="F40" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G40" s="67" t="n">
         <f aca="false">COUNTIF(N40:HA40,1)+COUNTIF(N40:HA40,2)*0.5</f>
@@ -39577,20 +39580,20 @@
     </row>
     <row r="41" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C41" s="79" t="n">
         <f aca="false">IF(OR(H41&lt;=1,I41&lt;=1)=1,0,IF(OR(H41&lt;2,I41&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F41" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G41" s="67" t="n">
         <f aca="false">COUNTIF(N41:HA41,1)+COUNTIF(N41:HA41,2)*0.5</f>
@@ -40157,10 +40160,10 @@
     </row>
     <row r="42" s="71" customFormat="true" ht="44.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="60" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B42" s="61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C42" s="79"/>
       <c r="D42" s="69"/>
@@ -40719,20 +40722,20 @@
     </row>
     <row r="43" customFormat="false" ht="54.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C43" s="79" t="n">
         <f aca="false">IF(OR(H43&lt;=1,I43&lt;=1)=1,0,IF(OR(H43&lt;2,I43&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F43" s="48" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G43" s="67" t="n">
         <f aca="false">COUNTIF(N43:HA43,1)+COUNTIF(N43:HA43,2)*0.5</f>
@@ -41299,10 +41302,10 @@
     </row>
     <row r="44" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C44" s="79" t="n">
         <f aca="false">IF(OR(H44&lt;=1,I44&lt;=1)=1,0,IF(OR(H44&lt;2,I44&lt;2)=1,1,2))</f>
@@ -41312,7 +41315,7 @@
         <v>118</v>
       </c>
       <c r="F44" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G44" s="67" t="n">
         <f aca="false">COUNTIF(N44:HA44,1)+COUNTIF(N44:HA44,2)*0.5</f>
@@ -41877,12 +41880,12 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C45" s="79" t="n">
         <f aca="false">IF(OR(H45&lt;=1,I45&lt;=1)=1,0,IF(OR(H45&lt;2,I45&lt;2)=1,1,2))</f>
@@ -42453,12 +42456,12 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="83" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B46" s="84" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C46" s="79" t="n">
         <f aca="false">IF(OR(H46&lt;=1,I46&lt;=1)=1,0,IF(OR(H46&lt;2,I46&lt;2)=1,1,2))</f>
@@ -43031,19 +43034,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="83" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B47" s="84" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C47" s="79" t="n">
         <f aca="false">IF(OR(H47&lt;=1,I47&lt;=1)=1,0,IF(OR(H47&lt;2,I47&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F47" s="48"/>
       <c r="G47" s="67" t="n">
@@ -43609,19 +43612,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="83" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B48" s="84" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C48" s="79" t="n">
         <f aca="false">IF(OR(H48&lt;=1,I48&lt;=1)=1,0,IF(OR(H48&lt;2,I48&lt;2)=1,1,2))</f>
         <v>1</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F48" s="48"/>
       <c r="G48" s="67" t="n">
@@ -44187,12 +44190,12 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="83" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B49" s="84" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C49" s="79" t="n">
         <f aca="false">IF(OR(H49&lt;=1,I49&lt;=1)=1,0,IF(OR(H49&lt;2,I49&lt;2)=1,1,2))</f>
@@ -44765,19 +44768,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="83" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B50" s="84" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C50" s="79" t="n">
         <f aca="false">IF(OR(H50&lt;=1,I50&lt;=1)=1,0,IF(OR(H50&lt;2,I50&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F50" s="48"/>
       <c r="G50" s="67" t="n">
@@ -45331,19 +45334,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="83" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B51" s="84" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C51" s="79" t="n">
         <f aca="false">IF(OR(H51&lt;=1,I51&lt;=1)=1,0,IF(OR(H51&lt;2,I51&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F51" s="48"/>
       <c r="G51" s="67" t="n">
@@ -45909,12 +45912,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="83" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B52" s="84" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C52" s="79" t="n">
         <f aca="false">IF(OR(H52&lt;=1,I52&lt;=1)=1,0,IF(OR(H52&lt;2,I52&lt;2)=1,1,2))</f>
@@ -46487,19 +46490,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="83" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B53" s="84" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C53" s="79" t="n">
         <f aca="false">IF(OR(H53&lt;=1,I53&lt;=1)=1,0,IF(OR(H53&lt;2,I53&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F53" s="48"/>
       <c r="G53" s="67" t="n">
@@ -47065,19 +47068,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="37.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="83" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B54" s="84" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C54" s="79" t="n">
         <f aca="false">IF(OR(H54&lt;=1,I54&lt;=1)=1,0,IF(OR(H54&lt;2,I54&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F54" s="48"/>
       <c r="G54" s="67" t="n">
@@ -47645,17 +47648,17 @@
     </row>
     <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="83" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B55" s="84" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C55" s="79" t="n">
         <f aca="false">IF(OR(H55&lt;=1,I55&lt;=1)=1,0,IF(OR(H55&lt;2,I55&lt;2)=1,1,2))</f>
         <v>1</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F55" s="48"/>
       <c r="G55" s="67" t="n">
@@ -48223,17 +48226,17 @@
     </row>
     <row r="56" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="83" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B56" s="84" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C56" s="79" t="n">
         <f aca="false">IF(OR(H56&lt;=1,I56&lt;=1)=1,0,IF(OR(H56&lt;2,I56&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F56" s="48"/>
       <c r="G56" s="67" t="n">
@@ -48801,17 +48804,17 @@
     </row>
     <row r="57" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="83" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B57" s="84" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C57" s="79" t="n">
         <f aca="false">IF(OR(H57&lt;=1,I57&lt;=1)=1,0,IF(OR(H57&lt;2,I57&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F57" s="48"/>
       <c r="G57" s="67" t="n">
@@ -49379,10 +49382,10 @@
     </row>
     <row r="58" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C58" s="79" t="n">
         <f aca="false">IF(OR(H58&lt;=1,I58&lt;=1)=1,0,IF(OR(H58&lt;2,I58&lt;2)=1,1,2))</f>
@@ -49957,17 +49960,17 @@
     </row>
     <row r="59" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C59" s="79" t="n">
         <f aca="false">IF(OR(H59&lt;=1,I59&lt;=1)=1,0,IF(OR(H59&lt;2,I59&lt;2)=1,1,2))</f>
         <v>1</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F59" s="48"/>
       <c r="G59" s="67" t="n">
@@ -50535,17 +50538,17 @@
     </row>
     <row r="60" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C60" s="79" t="n">
         <f aca="false">IF(OR(H60&lt;=1,I60&lt;=1)=1,0,IF(OR(H60&lt;2,I60&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F60" s="48"/>
       <c r="G60" s="67" t="n">
@@ -51113,17 +51116,17 @@
     </row>
     <row r="61" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C61" s="79" t="n">
         <f aca="false">IF(OR(H61&lt;=1,I61&lt;=1)=1,0,IF(OR(H61&lt;2,I61&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F61" s="48"/>
       <c r="G61" s="67" t="n">
@@ -51691,10 +51694,10 @@
     </row>
     <row r="62" s="71" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="60" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B62" s="61" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C62" s="79"/>
       <c r="D62" s="69"/>
@@ -52250,10 +52253,10 @@
     </row>
     <row r="63" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C63" s="79" t="n">
         <f aca="false">IF(OR(H63&lt;=1,I63&lt;=1)=1,0,IF(OR(H63&lt;2,I63&lt;2)=1,1,2))</f>
@@ -52263,7 +52266,7 @@
         <v>118</v>
       </c>
       <c r="F63" s="48" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G63" s="67" t="n">
         <f aca="false">COUNTIF(N63:HA63,1)+COUNTIF(N63:HA63,2)*0.5</f>
@@ -52800,19 +52803,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="54.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C64" s="79" t="n">
         <f aca="false">IF(OR(H64&lt;=1,I64&lt;=1)=1,0,IF(OR(H64&lt;2,I64&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F64" s="48"/>
       <c r="G64" s="67" t="n">
@@ -53352,10 +53355,10 @@
     </row>
     <row r="65" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="14" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C65" s="79" t="n">
         <f aca="false">IF(OR(H65&lt;=1,I65&lt;=1)=1,0,IF(OR(H65&lt;2,I65&lt;2)=1,1,2))</f>
@@ -53365,7 +53368,7 @@
         <v>118</v>
       </c>
       <c r="F65" s="48" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G65" s="67" t="n">
         <f aca="false">COUNTIF(N65:HA65,1)+COUNTIF(N65:HA65,2)*0.5</f>
@@ -53902,19 +53905,19 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="14" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C66" s="79" t="n">
         <f aca="false">IF(OR(H66&lt;=1,I66&lt;=1)=1,0,IF(OR(H66&lt;2,I66&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F66" s="48"/>
       <c r="G66" s="67" t="n">
@@ -54452,19 +54455,19 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="14" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C67" s="79" t="n">
         <f aca="false">IF(OR(H67&lt;=1,I67&lt;=1)=1,0,IF(OR(H67&lt;2,I67&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F67" s="48"/>
       <c r="G67" s="67" t="n">
@@ -55004,20 +55007,20 @@
     </row>
     <row r="68" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="14" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C68" s="79" t="n">
         <f aca="false">IF(OR(H68&lt;=1,I68&lt;=1)=1,0,IF(OR(H68&lt;2,I68&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F68" s="48" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="G68" s="67" t="n">
         <f aca="false">COUNTIF(N68:HA68,1)+COUNTIF(N68:HA68,2)*0.5</f>
@@ -55554,22 +55557,22 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="14" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C69" s="79" t="n">
         <f aca="false">IF(OR(H69&lt;=1,I69&lt;=1)=1,0,IF(OR(H69&lt;2,I69&lt;2)=1,1,2))</f>
         <v>0</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F69" s="48" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G69" s="67" t="n">
         <f aca="false">COUNTIF(N69:HA69,1)+COUNTIF(N69:HA69,2)*0.5</f>
@@ -56106,12 +56109,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C70" s="79" t="n">
         <f aca="false">IF(OR(H70&lt;=1,I70&lt;=1)=1,0,IF(OR(H70&lt;2,I70&lt;2)=1,1,2))</f>
@@ -56654,22 +56657,22 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C71" s="79" t="n">
         <f aca="false">IF(OR(H71&lt;=1,I71&lt;=1)=1,0,IF(OR(H71&lt;2,I71&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D71" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F71" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G71" s="67" t="n">
         <f aca="false">COUNTIF(N71:HA71,1)+COUNTIF(N71:HA71,2)*0.5</f>
@@ -57208,20 +57211,20 @@
     </row>
     <row r="72" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="14" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C72" s="79" t="n">
         <f aca="false">IF(OR(H72&lt;=1,I72&lt;=1)=1,0,IF(OR(H72&lt;2,I72&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D72" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F72" s="48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G72" s="67" t="n">
         <f aca="false">COUNTIF(N72:HA72,1)+COUNTIF(N72:HA72,2)*0.5</f>
@@ -57760,10 +57763,10 @@
     </row>
     <row r="73" s="71" customFormat="true" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="60" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B73" s="61" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C73" s="79"/>
       <c r="D73" s="69"/>
@@ -58319,20 +58322,20 @@
     </row>
     <row r="74" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C74" s="79" t="n">
         <f aca="false">IF(OR(H74&lt;=1,I74&lt;=1)=1,0,IF(OR(H74&lt;2,I74&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D74" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F74" s="48" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="G74" s="67" t="n">
         <f aca="false">COUNTIF(N74:HA74,1)+COUNTIF(N74:HA74,2)*0.5</f>
@@ -58871,20 +58874,20 @@
     </row>
     <row r="75" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C75" s="79" t="n">
         <f aca="false">IF(OR(H75&lt;=1,I75&lt;=1)=1,0,IF(OR(H75&lt;2,I75&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D75" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F75" s="48" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="G75" s="67" t="n">
         <f aca="false">COUNTIF(N75:HA75,1)+COUNTIF(N75:HA75,2)*0.5</f>
@@ -59423,20 +59426,20 @@
     </row>
     <row r="76" customFormat="false" ht="41.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="14" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="C76" s="79" t="n">
         <f aca="false">IF(OR(H76&lt;=1,I76&lt;=1)=1,0,IF(OR(H76&lt;2,I76&lt;2)=1,1,2))</f>
         <v>2</v>
       </c>
       <c r="D76" s="48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F76" s="48" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="G76" s="67" t="n">
         <f aca="false">COUNTIF(N76:HA76,1)+COUNTIF(N76:HA76,2)*0.5</f>
@@ -59973,10 +59976,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="87"/>
-      <c r="N77" s="88"/>
-    </row>
+    <row r="1048361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -66020,7 +66022,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{40DC7577-32A2-434A-90E4-B71EA492AF92}</x14:id>
+          <x14:id>{CE4E321C-DC85-482E-9953-E4C82E2C9AA6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -66034,7 +66036,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2AD910C0-6A84-4DCE-93B7-AD4419F78CEC}</x14:id>
+          <x14:id>{E429243F-2466-49E1-8116-347CB526BECA}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -66048,7 +66050,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D2CA829D-9575-4045-98F2-E826B7D3B9EA}</x14:id>
+          <x14:id>{1AFA3B25-D253-4AA0-8365-D64FC7B138C1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -66073,7 +66075,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{40DC7577-32A2-434A-90E4-B71EA492AF92}">
+          <x14:cfRule type="dataBar" id="{CE4E321C-DC85-482E-9953-E4C82E2C9AA6}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -66084,7 +66086,7 @@
           <xm:sqref>G:G</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2AD910C0-6A84-4DCE-93B7-AD4419F78CEC}">
+          <x14:cfRule type="dataBar" id="{E429243F-2466-49E1-8116-347CB526BECA}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -66095,7 +66097,7 @@
           <xm:sqref>H:H</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D2CA829D-9575-4045-98F2-E826B7D3B9EA}">
+          <x14:cfRule type="dataBar" id="{1AFA3B25-D253-4AA0-8365-D64FC7B138C1}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -66106,7 +66108,7 @@
           <xm:sqref>I:I</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1497" id="{305C3295-A537-4121-B25B-3AAE00CB751C}">
+          <x14:cfRule type="iconSet" priority="1497" id="{9D43BB8B-7849-48F1-9F63-CED0792D89B0}">
             <x14:iconSet iconSet="3Triangles" custom="1" reverse="0" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>

</xml_diff>